<commit_message>
Implemented RFID module with Arduino. Integrated system
</commit_message>
<xml_diff>
--- a/files/mapping.xlsx
+++ b/files/mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year3Sem2\IS4151\Assignments\Assignments\Group Project\Repos\PI-Edge\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06EECAD-C9F1-4C86-8C11-9AF3566FE718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DEA8AB-B0BA-4EF3-89CE-25F00B316F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>getit</t>
-  </si>
-  <si>
     <t>CART_001</t>
   </si>
   <si>
@@ -54,24 +51,6 @@
     <t>item</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>MP1WsknTkMqlvom70wDq</t>
   </si>
   <si>
@@ -100,6 +79,27 @@
   </si>
   <si>
     <t>CART_003</t>
+  </si>
+  <si>
+    <t>C7E671B4</t>
+  </si>
+  <si>
+    <t>0A4B997F</t>
+  </si>
+  <si>
+    <t>AAAAAAA</t>
+  </si>
+  <si>
+    <t>BBBBBBBB</t>
+  </si>
+  <si>
+    <t>CCCCCCCC</t>
+  </si>
+  <si>
+    <t>DDDDDDDD</t>
+  </si>
+  <si>
+    <t>zovag</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,34 +487,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -530,68 +530,69 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated mapping to prototype cart
</commit_message>
<xml_diff>
--- a/files/mapping.xlsx
+++ b/files/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year3Sem2\IS4151\Assignments\Assignments\Group Project\Repos\PI-Edge\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DEA8AB-B0BA-4EF3-89CE-25F00B316F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C0728D-764B-4C13-8770-FF5F99E7074F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
   </bookViews>
   <sheets>
     <sheet name="device_cart" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
     <t>DDDDDDDD</t>
   </si>
   <si>
-    <t>zovag</t>
+    <t>getit</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D3DA47-3878-44FA-A4FD-95B03017DBDE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -529,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1211525-CD61-4C18-8915-77DBC03DDA13}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added serial testing script
</commit_message>
<xml_diff>
--- a/files/mapping.xlsx
+++ b/files/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year3Sem2\IS4151\Assignments\Assignments\Group Project\Repos\PI-Edge\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C0728D-764B-4C13-8770-FF5F99E7074F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F040370-1E21-476C-AE6E-04C50BAACEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
   </bookViews>
   <sheets>
     <sheet name="device_cart" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>CART_001</t>
   </si>
@@ -87,9 +87,6 @@
     <t>0A4B997F</t>
   </si>
   <si>
-    <t>AAAAAAA</t>
-  </si>
-  <si>
     <t>BBBBBBBB</t>
   </si>
   <si>
@@ -99,7 +96,22 @@
     <t>DDDDDDDD</t>
   </si>
   <si>
-    <t>getit</t>
+    <t>gugug</t>
+  </si>
+  <si>
+    <t>D792AD2D</t>
+  </si>
+  <si>
+    <t>B8B03D1E</t>
+  </si>
+  <si>
+    <t>AAAAAAAA</t>
+  </si>
+  <si>
+    <t>RMWLUuACH72OuqSPYQDk</t>
+  </si>
+  <si>
+    <t>rxRod7cigQjBK9dDmlHv</t>
   </si>
 </sst>
 </file>
@@ -166,8 +178,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6D7ABB5-B723-4EBB-943E-647A01FA6E87}" name="Table2" displayName="Table2" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{D4826BC7-EA6B-4038-8449-EB4AE371C27F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6D7ABB5-B723-4EBB-943E-647A01FA6E87}" name="Table2" displayName="Table2" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{D4826BC7-EA6B-4038-8449-EB4AE371C27F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D879BA87-0C03-4D11-93C3-DC39824C03E5}" name="rfid"/>
     <tableColumn id="2" xr3:uid="{71A2D2D0-15D4-4A57-87D3-3E5B32CC61AE}" name="item"/>
@@ -475,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D3DA47-3878-44FA-A4FD-95B03017DBDE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -495,7 +507,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -527,15 +539,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1211525-CD61-4C18-8915-77DBC03DDA13}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -557,7 +569,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -565,7 +577,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -573,26 +585,42 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
endpoint accepts item param and position adjustment impl-ed
</commit_message>
<xml_diff>
--- a/files/mapping.xlsx
+++ b/files/mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year3Sem2\IS4151\Assignments\Assignments\Group Project\Repos\PI-Edge\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F040370-1E21-476C-AE6E-04C50BAACEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887DB8D1-54E5-4F9B-B2DF-DF3EB17A107F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>CART_001</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>rxRod7cigQjBK9dDmlHv</t>
+  </si>
+  <si>
+    <t>EEEEEEEE</t>
   </si>
 </sst>
 </file>
@@ -178,8 +181,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6D7ABB5-B723-4EBB-943E-647A01FA6E87}" name="Table2" displayName="Table2" ref="A1:B9" totalsRowShown="0">
-  <autoFilter ref="A1:B9" xr:uid="{D4826BC7-EA6B-4038-8449-EB4AE371C27F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6D7ABB5-B723-4EBB-943E-647A01FA6E87}" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{D4826BC7-EA6B-4038-8449-EB4AE371C27F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D879BA87-0C03-4D11-93C3-DC39824C03E5}" name="rfid"/>
     <tableColumn id="2" xr3:uid="{71A2D2D0-15D4-4A57-87D3-3E5B32CC61AE}" name="item"/>
@@ -539,10 +542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1211525-CD61-4C18-8915-77DBC03DDA13}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +591,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +599,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +607,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +615,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,6 +623,14 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added items into mapping, updated arduino to be compatible with NTags
</commit_message>
<xml_diff>
--- a/files/mapping.xlsx
+++ b/files/mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year3Sem2\IS4151\Assignments\Assignments\Group Project\Repos\PI-Edge\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887DB8D1-54E5-4F9B-B2DF-DF3EB17A107F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618C32D1-8087-439E-A130-994ABDB9587D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
+    <workbookView xWindow="6090" yWindow="-15360" windowWidth="18135" windowHeight="11385" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
   </bookViews>
   <sheets>
     <sheet name="device_cart" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>CART_001</t>
   </si>
@@ -87,15 +87,6 @@
     <t>0A4B997F</t>
   </si>
   <si>
-    <t>BBBBBBBB</t>
-  </si>
-  <si>
-    <t>CCCCCCCC</t>
-  </si>
-  <si>
-    <t>DDDDDDDD</t>
-  </si>
-  <si>
     <t>gugug</t>
   </si>
   <si>
@@ -105,16 +96,37 @@
     <t>B8B03D1E</t>
   </si>
   <si>
-    <t>AAAAAAAA</t>
-  </si>
-  <si>
     <t>RMWLUuACH72OuqSPYQDk</t>
   </si>
   <si>
     <t>rxRod7cigQjBK9dDmlHv</t>
   </si>
   <si>
-    <t>EEEEEEEE</t>
+    <t>049B4B22</t>
+  </si>
+  <si>
+    <t>049F4B22</t>
+  </si>
+  <si>
+    <t>04974B22</t>
+  </si>
+  <si>
+    <t>04934B22</t>
+  </si>
+  <si>
+    <t>048F4B22</t>
+  </si>
+  <si>
+    <t>048B4B22</t>
+  </si>
+  <si>
+    <t>04874B22</t>
+  </si>
+  <si>
+    <t>04834B22</t>
+  </si>
+  <si>
+    <t>047F4B22</t>
   </si>
 </sst>
 </file>
@@ -181,8 +193,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6D7ABB5-B723-4EBB-943E-647A01FA6E87}" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10" xr:uid="{D4826BC7-EA6B-4038-8449-EB4AE371C27F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6D7ABB5-B723-4EBB-943E-647A01FA6E87}" name="Table2" displayName="Table2" ref="A1:B14" totalsRowShown="0">
+  <autoFilter ref="A1:B14" xr:uid="{D4826BC7-EA6B-4038-8449-EB4AE371C27F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D879BA87-0C03-4D11-93C3-DC39824C03E5}" name="rfid"/>
     <tableColumn id="2" xr3:uid="{71A2D2D0-15D4-4A57-87D3-3E5B32CC61AE}" name="item"/>
@@ -490,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D3DA47-3878-44FA-A4FD-95B03017DBDE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +522,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -542,10 +554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1211525-CD61-4C18-8915-77DBC03DDA13}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +584,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -580,7 +592,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -596,15 +608,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -612,18 +624,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -631,7 +643,39 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
post demo code updates
</commit_message>
<xml_diff>
--- a/files/mapping.xlsx
+++ b/files/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year3Sem2\IS4151\Assignments\Assignments\Group Project\Repos\PI-Edge\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618C32D1-8087-439E-A130-994ABDB9587D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D534536-2EC0-4BE4-A9C7-FD52D70F166C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="-15360" windowWidth="18135" windowHeight="11385" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{E5C48810-216C-455B-B709-CA52318FDEA7}"/>
   </bookViews>
   <sheets>
     <sheet name="device_cart" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>CART_001</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>YvxptylcQC7o6s7fK7H9</t>
-  </si>
-  <si>
-    <t>oZGiQLJMymfo2Mc4KJYm</t>
-  </si>
-  <si>
-    <t>VfgrHcX6LvHuAvkJtdgU</t>
   </si>
   <si>
     <t>pipov</t>
@@ -162,8 +156,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D3DA47-3878-44FA-A4FD-95B03017DBDE}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +507,7 @@
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -520,29 +515,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -556,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1211525-CD61-4C18-8915-77DBC03DDA13}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +574,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -584,7 +582,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -592,7 +590,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -600,7 +598,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -608,74 +606,74 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>